<commit_message>
SD-80254 - CCRU - Wrong KPI target fixed
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Small - CAP.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Small - CAP.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Convenience Small'!$A$1:$AL$169</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Convenience Small'!$A$1:$AL$169</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Convenience Small'!$A$1:$AL$169</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Convenience Small'!$A$1:$AL$169</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2269,52 +2270,52 @@
   </sheetPr>
   <dimension ref="A1:AL169"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
-      <selection pane="bottomLeft" activeCell="X142" activeCellId="0" sqref="X142:X143"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A125" activeCellId="0" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2793522267206"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="68.7692307692308"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="50.668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.8461538461539"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="69.412955465587"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="60.8421052631579"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="61.3805668016194"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="88.1578947368421"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="127.14979757085"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="56.2388663967611"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="26.8866396761134"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="88.9068825910931"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="128.222672064777"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="56.663967611336"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="27.1012145748988"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="32" min="32" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="64.2712550607287"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="64.8056680161943"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.03238866396761"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
@@ -11583,7 +11584,7 @@
       </c>
       <c r="I121" s="5"/>
       <c r="J121" s="7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K121" s="7"/>
       <c r="L121" s="7"/>

</xml_diff>